<commit_message>
Change point detection algorithm
</commit_message>
<xml_diff>
--- a/results/3r/camera_calibration_.xlsx
+++ b/results/3r/camera_calibration_.xlsx
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>C23F07_upd</t>
+          <t>C23F07</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -517,7 +517,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>C24F07_upd</t>
+          <t>C24F07</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -551,7 +551,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>C25F07_upd</t>
+          <t>C25F07</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -585,7 +585,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>C26Finf_upd</t>
+          <t>C26Finf</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -619,7 +619,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>C27Finf_upd</t>
+          <t>C27Finf</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -653,7 +653,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>C28Finf_upd</t>
+          <t>C28Finf</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -687,7 +687,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>C29FInf_upd</t>
+          <t>C29Finf</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -721,7 +721,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>C30FInf_upd</t>
+          <t>C30Finf</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -755,7 +755,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>C31FInf_upd</t>
+          <t>C31Finf</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -789,7 +789,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>C32Finf_upd</t>
+          <t>C32Finf</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -823,7 +823,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>C33Finf_upd</t>
+          <t>C33Finf</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -857,7 +857,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>C34Finf_upd</t>
+          <t>C34Finf</t>
         </is>
       </c>
       <c r="B13" t="n">

</xml_diff>